<commit_message>
Replace DataTable with IEnumerabe
</commit_message>
<xml_diff>
--- a/Tests/ExcelTemplates/Basic.xlsx
+++ b/Tests/ExcelTemplates/Basic.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="NamedCell">Tabelle1!$C$4</definedName>
+    <definedName name="NameCell" localSheetId="0">Tabelle1!$C$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -370,7 +370,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>